<commit_message>
fix voor url's in RdwDienst
</commit_message>
<xml_diff>
--- a/MDT/RollenEnBeheerdersPassen/adfsEenheden.xlsx
+++ b/MDT/RollenEnBeheerdersPassen/adfsEenheden.xlsx
@@ -7995,10 +7995,10 @@
   <dimension ref="A1:D86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8033,8 +8033,8 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
-        <f>"https://"&amp;B3&amp;"/"</f>
-        <v>https://oreh.rdw.nl/</v>
+        <f t="shared" ref="A3:A66" si="0">"https%3A%2F%2F"&amp;SUBSTITUTE(B3,"/","%2F")&amp;"%2F"</f>
+        <v>https%3A%2F%2Foreh.rdw.nl%2F</v>
       </c>
       <c r="B3" t="s">
         <v>122</v>
@@ -8046,8 +8046,8 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
-        <f t="shared" ref="A4:A67" si="0">"https://"&amp;B4&amp;"/"</f>
-        <v>https://orb.rdw.nl/</v>
+        <f t="shared" si="0"/>
+        <v>https%3A%2F%2Forb.rdw.nl%2F</v>
       </c>
       <c r="B4" t="s">
         <v>123</v>
@@ -8060,7 +8060,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
-        <v>https://rtl.rdw.nl/</v>
+        <v>https%3A%2F%2Frtl.rdw.nl%2F</v>
       </c>
       <c r="B5" t="s">
         <v>124</v>
@@ -8073,7 +8073,7 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
-        <v>https://hhwuitsluitensvc.rdw.nl/</v>
+        <v>https%3A%2F%2Fhhwuitsluitensvc.rdw.nl%2F</v>
       </c>
       <c r="B6" t="s">
         <v>125</v>
@@ -8086,7 +8086,7 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
-        <v>https://alpsvc.rdw.nl/</v>
+        <v>https%3A%2F%2Falpsvc.rdw.nl%2F</v>
       </c>
       <c r="B7" t="s">
         <v>126</v>
@@ -8099,7 +8099,7 @@
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
-        <v>https://katv.rdw.nl/</v>
+        <v>https%3A%2F%2Fkatv.rdw.nl%2F</v>
       </c>
       <c r="B8" t="s">
         <v>127</v>
@@ -8112,7 +8112,7 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
-        <v>https://apk.rdw.nl/</v>
+        <v>https%3A%2F%2Fapk.rdw.nl%2F</v>
       </c>
       <c r="B9" t="s">
         <v>128</v>
@@ -8125,7 +8125,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
-        <v>https://rme.rdw.nl/</v>
+        <v>https%3A%2F%2Frme.rdw.nl%2F</v>
       </c>
       <c r="B10" t="s">
         <v>161</v>
@@ -8138,7 +8138,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
-        <v>https://eucop.rdw.nl/</v>
+        <v>https%3A%2F%2Feucop.rdw.nl%2F</v>
       </c>
       <c r="B11" t="s">
         <v>129</v>
@@ -8151,7 +8151,7 @@
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
-        <v>https://eucaris.rdw.nl/</v>
+        <v>https%3A%2F%2Feucaris.rdw.nl%2F</v>
       </c>
       <c r="B12" t="s">
         <v>130</v>
@@ -8164,7 +8164,7 @@
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
-        <v>https://standcodering.rdw.nl/</v>
+        <v>https%3A%2F%2Fstandcodering.rdw.nl%2F</v>
       </c>
       <c r="B13" t="s">
         <v>133</v>
@@ -8177,7 +8177,7 @@
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
-        <v>https://keurmeesterinformatie.rdw.nl/</v>
+        <v>https%3A%2F%2Fkeurmeesterinformatie.rdw.nl%2F</v>
       </c>
       <c r="B14" t="s">
         <v>131</v>
@@ -8190,7 +8190,7 @@
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
-        <v>https://webrme.rdw.nl/</v>
+        <v>https%3A%2F%2Fwebrme.rdw.nl%2F</v>
       </c>
       <c r="B15" t="s">
         <v>132</v>
@@ -8203,7 +8203,7 @@
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
-        <v>https://www-a.rdw.nl/_trust/</v>
+        <v>https%3A%2F%2Fwww-a.rdw.nl%2F_trust%2F</v>
       </c>
       <c r="B16" t="s">
         <v>163</v>
@@ -8216,7 +8216,7 @@
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
-        <v>https://federatie.rdw.nl/</v>
+        <v>https%3A%2F%2Ffederatie.rdw.nl%2F</v>
       </c>
       <c r="B17" t="s">
         <v>135</v>
@@ -8229,7 +8229,7 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
-        <v>https://mijnvoertuig.rdw.nl/</v>
+        <v>https%3A%2F%2Fmijnvoertuig.rdw.nl%2F</v>
       </c>
       <c r="B18" t="s">
         <v>136</v>
@@ -8242,7 +8242,7 @@
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
-        <v>https://schorsen.rdw.nl/schorsen/</v>
+        <v>https%3A%2F%2Fschorsen.rdw.nl%2Fschorsen%2F</v>
       </c>
       <c r="B19" t="s">
         <v>137</v>
@@ -8255,7 +8255,7 @@
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
-        <v>https://berichtenbox.rdw.nl/</v>
+        <v>https%3A%2F%2Fberichtenbox.rdw.nl%2F</v>
       </c>
       <c r="B20" t="s">
         <v>138</v>
@@ -8268,7 +8268,7 @@
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
-        <v>https://burger.rdw.nl/</v>
+        <v>https%3A%2F%2Fburger.rdw.nl%2F</v>
       </c>
       <c r="B21" t="s">
         <v>139</v>
@@ -8281,7 +8281,7 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
-        <v>https://vvkbedrijven.rdw.nl/vvkb/</v>
+        <v>https%3A%2F%2Fvvkbedrijven.rdw.nl%2Fvvkb%2F</v>
       </c>
       <c r="B22" t="s">
         <v>140</v>
@@ -8294,7 +8294,7 @@
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
-        <v>https://bedrijf.rdw.nl/</v>
+        <v>https%3A%2F%2Fbedrijf.rdw.nl%2F</v>
       </c>
       <c r="B23" t="s">
         <v>141</v>
@@ -8307,7 +8307,7 @@
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
-        <v>https://berichtenbox.rdw.nl/RDW.GEXXX/</v>
+        <v>https%3A%2F%2Fberichtenbox.rdw.nl%2FRDW.GEXXX%2F</v>
       </c>
       <c r="B24" t="s">
         <v>142</v>
@@ -8320,7 +8320,7 @@
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
-        <v>https://bvo.rdw.nl/bvo/</v>
+        <v>https%3A%2F%2Fbvo.rdw.nl%2Fbvo%2F</v>
       </c>
       <c r="B25" t="s">
         <v>143</v>
@@ -8333,7 +8333,7 @@
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
-        <v>https://rer.rdw.nl/</v>
+        <v>https%3A%2F%2Frer.rdw.nl%2F</v>
       </c>
       <c r="B26" t="s">
         <v>144</v>
@@ -8346,7 +8346,7 @@
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
-        <v>https://tvbedrijf.rdw.nl/</v>
+        <v>https%3A%2F%2Ftvbedrijf.rdw.nl%2F</v>
       </c>
       <c r="B27" t="s">
         <v>145</v>
@@ -8359,7 +8359,7 @@
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
-        <v>https://tmv.rdw.nl/</v>
+        <v>https%3A%2F%2Ftmv.rdw.nl%2F</v>
       </c>
       <c r="B28" t="s">
         <v>146</v>
@@ -8372,7 +8372,7 @@
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
-        <v>https://crosweb.rdw.nl/</v>
+        <v>https%3A%2F%2Fcrosweb.rdw.nl%2F</v>
       </c>
       <c r="B29" t="s">
         <v>147</v>
@@ -8385,7 +8385,7 @@
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
-        <v>https://dnt.rdw.nl/</v>
+        <v>https%3A%2F%2Fdnt.rdw.nl%2F</v>
       </c>
       <c r="B30" t="s">
         <v>148</v>
@@ -8398,7 +8398,7 @@
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
-        <v>https://rpvbeheer.rdw.nl/</v>
+        <v>https%3A%2F%2Frpvbeheer.rdw.nl%2F</v>
       </c>
       <c r="B31" t="s">
         <v>149</v>
@@ -8411,7 +8411,7 @@
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
-        <v>https://digitalekluis.rdw.nl/</v>
+        <v>https%3A%2F%2Fdigitalekluis.rdw.nl%2F</v>
       </c>
       <c r="B32" t="s">
         <v>150</v>
@@ -8424,7 +8424,7 @@
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
-        <v>https://intsvcportalsssp.rdw.nl/</v>
+        <v>https%3A%2F%2Fintsvcportalsssp.rdw.nl%2F</v>
       </c>
       <c r="B33" t="s">
         <v>151</v>
@@ -8437,7 +8437,7 @@
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
-        <v>https://rpvinfo.rdw.nl/</v>
+        <v>https%3A%2F%2Frpvinfo.rdw.nl%2F</v>
       </c>
       <c r="B34" t="s">
         <v>152</v>
@@ -8450,7 +8450,7 @@
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
-        <v>https://radar.rdw.nl/</v>
+        <v>https%3A%2F%2Fradar.rdw.nl%2F</v>
       </c>
       <c r="B35" t="s">
         <v>153</v>
@@ -8463,7 +8463,7 @@
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
-        <v>https://gob.rdw.nl/</v>
+        <v>https%3A%2F%2Fgob.rdw.nl%2F</v>
       </c>
       <c r="B36" t="s">
         <v>154</v>
@@ -8476,7 +8476,7 @@
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
-        <v>https://epb.rdw.nl/</v>
+        <v>https%3A%2F%2Fepb.rdw.nl%2F</v>
       </c>
       <c r="B37" t="s">
         <v>31</v>
@@ -8489,7 +8489,7 @@
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
-        <v>https://lpb.rdw.nl/_trust/</v>
+        <v>https%3A%2F%2Flpb.rdw.nl%2F_trust%2F</v>
       </c>
       <c r="B38" t="s">
         <v>155</v>
@@ -8502,7 +8502,7 @@
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
-        <v>https://niwo.rdw.nl/</v>
+        <v>https%3A%2F%2Fniwo.rdw.nl%2F</v>
       </c>
       <c r="B39" t="s">
         <v>156</v>
@@ -8515,7 +8515,7 @@
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
-        <v>https://webcnb.rdw.nl/</v>
+        <v>https%3A%2F%2Fwebcnb.rdw.nl%2F</v>
       </c>
       <c r="B40" t="s">
         <v>157</v>
@@ -8528,7 +8528,7 @@
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
         <f t="shared" si="0"/>
-        <v>https://webtrb.rdw.nl/</v>
+        <v>https%3A%2F%2Fwebtrb.rdw.nl%2F</v>
       </c>
       <c r="B41" t="s">
         <v>158</v>
@@ -8541,7 +8541,7 @@
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="str">
         <f t="shared" si="0"/>
-        <v>https://dienstenportaal.rdw.nl/_trust/</v>
+        <v>https%3A%2F%2Fdienstenportaal.rdw.nl%2F_trust%2F</v>
       </c>
       <c r="B42" t="s">
         <v>159</v>
@@ -8554,7 +8554,7 @@
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="str">
         <f t="shared" si="0"/>
-        <v>https://www.rdw.nl/_trust/</v>
+        <v>https%3A%2F%2Fwww.rdw.nl%2F_trust%2F</v>
       </c>
       <c r="B43" t="s">
         <v>160</v>
@@ -8567,7 +8567,7 @@
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="str">
         <f t="shared" si="0"/>
-        <v>https://webikr.rdw.nl/</v>
+        <v>https%3A%2F%2Fwebikr.rdw.nl%2F</v>
       </c>
       <c r="B44" t="s">
         <v>81</v>
@@ -8580,7 +8580,7 @@
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="str">
         <f t="shared" si="0"/>
-        <v>https://webrdd.rdw.nl/</v>
+        <v>https%3A%2F%2Fwebrdd.rdw.nl%2F</v>
       </c>
       <c r="B45" t="s">
         <v>82</v>
@@ -8593,7 +8593,7 @@
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="str">
         <f t="shared" si="0"/>
-        <v>https://recallregistratie.rdw.nl/</v>
+        <v>https%3A%2F%2Frecallregistratie.rdw.nl%2F</v>
       </c>
       <c r="B46" t="s">
         <v>83</v>
@@ -8606,7 +8606,7 @@
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="str">
         <f t="shared" si="0"/>
-        <v>https://webret.rdw.nl/</v>
+        <v>https%3A%2F%2Fwebret.rdw.nl%2F</v>
       </c>
       <c r="B47" t="s">
         <v>84</v>
@@ -8619,7 +8619,7 @@
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="str">
         <f t="shared" si="0"/>
-        <v>https://jaarverslag-a.rdw.nl/_trust/</v>
+        <v>https%3A%2F%2Fjaarverslag-a.rdw.nl%2F_trust%2F</v>
       </c>
       <c r="B48" t="s">
         <v>85</v>
@@ -8632,7 +8632,7 @@
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="str">
         <f t="shared" si="0"/>
-        <v>https://jaarverslag2010-a.rdw.nl/_trust/</v>
+        <v>https%3A%2F%2Fjaarverslag2010-a.rdw.nl%2F_trust%2F</v>
       </c>
       <c r="B49" t="s">
         <v>89</v>
@@ -8645,7 +8645,7 @@
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="str">
         <f t="shared" si="0"/>
-        <v>https://jaarverslag2011-a.rdw.nl/_trust/</v>
+        <v>https%3A%2F%2Fjaarverslag2011-a.rdw.nl%2F_trust%2F</v>
       </c>
       <c r="B50" t="s">
         <v>90</v>
@@ -8658,7 +8658,7 @@
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="str">
         <f t="shared" si="0"/>
-        <v>https://jaarverslag2012-a.rdw.nl/_trust/</v>
+        <v>https%3A%2F%2Fjaarverslag2012-a.rdw.nl%2F_trust%2F</v>
       </c>
       <c r="B51" t="s">
         <v>88</v>
@@ -8671,7 +8671,7 @@
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="str">
         <f t="shared" si="0"/>
-        <v>https://medewerker.rdw.nl/</v>
+        <v>https%3A%2F%2Fmedewerker.rdw.nl%2F</v>
       </c>
       <c r="B52" t="s">
         <v>91</v>
@@ -8684,7 +8684,7 @@
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="str">
         <f t="shared" si="0"/>
-        <v>https://handboek-a.rdw.nl/_trust/</v>
+        <v>https%3A%2F%2Fhandboek-a.rdw.nl%2F_trust%2F</v>
       </c>
       <c r="B53" t="s">
         <v>92</v>
@@ -8697,7 +8697,7 @@
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="str">
         <f t="shared" si="0"/>
-        <v>https://photocompare.rdw.nl/</v>
+        <v>https%3A%2F%2Fphotocompare.rdw.nl%2F</v>
       </c>
       <c r="B54" t="s">
         <v>93</v>
@@ -8710,7 +8710,7 @@
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="str">
         <f t="shared" si="0"/>
-        <v>https://gaikbeheer.rdw.nl/</v>
+        <v>https%3A%2F%2Fgaikbeheer.rdw.nl%2F</v>
       </c>
       <c r="B55" t="s">
         <v>94</v>
@@ -8723,7 +8723,7 @@
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="str">
         <f t="shared" si="0"/>
-        <v>https://orad.rdw.nl/</v>
+        <v>https%3A%2F%2Forad.rdw.nl%2F</v>
       </c>
       <c r="B56" t="s">
         <v>95</v>
@@ -8736,7 +8736,7 @@
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="str">
         <f t="shared" si="0"/>
-        <v>https://asp.rdw.nl/</v>
+        <v>https%3A%2F%2Fasp.rdw.nl%2F</v>
       </c>
       <c r="B57" t="s">
         <v>96</v>
@@ -8749,7 +8749,7 @@
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="str">
         <f t="shared" si="0"/>
-        <v>https://keys-asp.rdw.nl/</v>
+        <v>https%3A%2F%2Fkeys-asp.rdw.nl%2F</v>
       </c>
       <c r="B58" t="s">
         <v>97</v>
@@ -8762,7 +8762,7 @@
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="str">
         <f t="shared" si="0"/>
-        <v>https://dienstenportaal.rdw.nl/orders/</v>
+        <v>https%3A%2F%2Fdienstenportaal.rdw.nl%2Forders%2F</v>
       </c>
       <c r="B59" t="s">
         <v>98</v>
@@ -8775,7 +8775,7 @@
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="str">
         <f t="shared" si="0"/>
-        <v>https://rbcbedrijven.rdw.nl/</v>
+        <v>https%3A%2F%2Frbcbedrijven.rdw.nl%2F</v>
       </c>
       <c r="B60" t="s">
         <v>99</v>
@@ -8788,7 +8788,7 @@
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="str">
         <f t="shared" si="0"/>
-        <v>https://ovibedrijven.rdw.nl/</v>
+        <v>https%3A%2F%2Fovibedrijven.rdw.nl%2F</v>
       </c>
       <c r="B61" t="s">
         <v>100</v>
@@ -8801,7 +8801,7 @@
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="str">
         <f t="shared" si="0"/>
-        <v>https://webbrv.rdw.nl/</v>
+        <v>https%3A%2F%2Fwebbrv.rdw.nl%2F</v>
       </c>
       <c r="B62" t="s">
         <v>101</v>
@@ -8814,7 +8814,7 @@
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="str">
         <f t="shared" si="0"/>
-        <v>https://webmob.rdw.nl/</v>
+        <v>https%3A%2F%2Fwebmob.rdw.nl%2F</v>
       </c>
       <c r="B63" t="s">
         <v>102</v>
@@ -8827,7 +8827,7 @@
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="str">
         <f t="shared" si="0"/>
-        <v>https://ivibeheer.rdw.nl/</v>
+        <v>https%3A%2F%2Fivibeheer.rdw.nl%2F</v>
       </c>
       <c r="B64" t="s">
         <v>165</v>
@@ -8840,7 +8840,7 @@
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="str">
         <f t="shared" si="0"/>
-        <v>https://webrem.rdw.nl/</v>
+        <v>https%3A%2F%2Fwebrem.rdw.nl%2F</v>
       </c>
       <c r="B65" t="s">
         <v>103</v>
@@ -8853,7 +8853,7 @@
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="str">
         <f t="shared" si="0"/>
-        <v>https://vldbeheer.rdw.nl/</v>
+        <v>https%3A%2F%2Fvldbeheer.rdw.nl%2F</v>
       </c>
       <c r="B66" t="s">
         <v>104</v>
@@ -8865,8 +8865,8 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="str">
-        <f t="shared" si="0"/>
-        <v>https://webfwe.rdw.nl/</v>
+        <f t="shared" ref="A67:A77" si="1">"https%3A%2F%2F"&amp;SUBSTITUTE(B67,"/","%2F")&amp;"%2F"</f>
+        <v>https%3A%2F%2Fwebfwe.rdw.nl%2F</v>
       </c>
       <c r="B67" t="s">
         <v>105</v>
@@ -8878,8 +8878,8 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="str">
-        <f t="shared" ref="A68:A86" si="1">"https://"&amp;B68&amp;"/"</f>
-        <v>https://authenticatie2.rdw.nl/wifdemo4XXX/</v>
+        <f t="shared" si="1"/>
+        <v>https%3A%2F%2Fauthenticatie2.rdw.nl%2Fwifdemo4XXX%2F</v>
       </c>
       <c r="B68" t="s">
         <v>106</v>
@@ -8892,7 +8892,7 @@
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="str">
         <f t="shared" si="1"/>
-        <v>https://mtv.rdw.nl/</v>
+        <v>https%3A%2F%2Fmtv.rdw.nl%2F</v>
       </c>
       <c r="B69" t="s">
         <v>107</v>
@@ -8905,7 +8905,7 @@
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="str">
         <f t="shared" si="1"/>
-        <v>https://aks.rdw.nl/</v>
+        <v>https%3A%2F%2Faks.rdw.nl%2F</v>
       </c>
       <c r="B70" t="s">
         <v>108</v>
@@ -8918,7 +8918,7 @@
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="str">
         <f t="shared" si="1"/>
-        <v>https://jaarverslag2014-a.rdw.nl/_trust/</v>
+        <v>https%3A%2F%2Fjaarverslag2014-a.rdw.nl%2F_trust%2F</v>
       </c>
       <c r="B71" t="s">
         <v>87</v>
@@ -8931,7 +8931,7 @@
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="str">
         <f t="shared" si="1"/>
-        <v>https://afnorth.rdw.nl/</v>
+        <v>https%3A%2F%2Fafnorth.rdw.nl%2F</v>
       </c>
       <c r="B72" t="s">
         <v>109</v>
@@ -8944,7 +8944,7 @@
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="str">
         <f t="shared" si="1"/>
-        <v>https://Rdw-zaken.rdw.nl/_trust/</v>
+        <v>https%3A%2F%2FRdw-zaken.rdw.nl%2F_trust%2F</v>
       </c>
       <c r="B73" t="s">
         <v>110</v>
@@ -8957,7 +8957,7 @@
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="str">
         <f t="shared" si="1"/>
-        <v>https://webams.rdw.nl/</v>
+        <v>https%3A%2F%2Fwebams.rdw.nl%2F</v>
       </c>
       <c r="B74" t="s">
         <v>111</v>
@@ -8970,7 +8970,7 @@
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="str">
         <f t="shared" si="1"/>
-        <v>https://webcplus.rdw.nl/</v>
+        <v>https%3A%2F%2Fwebcplus.rdw.nl%2F</v>
       </c>
       <c r="B75" t="s">
         <v>112</v>
@@ -8983,7 +8983,7 @@
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="str">
         <f t="shared" si="1"/>
-        <v>https://webbrd.rdw.nl/</v>
+        <v>https%3A%2F%2Fwebbrd.rdw.nl%2F</v>
       </c>
       <c r="B76" t="s">
         <v>113</v>
@@ -8996,7 +8996,7 @@
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="str">
         <f t="shared" si="1"/>
-        <v>https://tv.rdw.nl/</v>
+        <v>https%3A%2F%2Ftv.rdw.nl%2F</v>
       </c>
       <c r="B77" t="s">
         <v>114</v>
@@ -9008,8 +9008,8 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="str">
-        <f t="shared" si="1"/>
-        <v>https://webvkr.rdw.nl/</v>
+        <f t="shared" ref="A78:A85" si="2">"https%3A%2F%2F"&amp;SUBSTITUTE(B78,"/","%2F")&amp;"%2F"</f>
+        <v>https%3A%2F%2Fwebvkr.rdw.nl%2F</v>
       </c>
       <c r="B78" t="s">
         <v>72</v>
@@ -9021,8 +9021,8 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="str">
-        <f t="shared" si="1"/>
-        <v>https://jaarverslag2013-a.rdw.nl/_trust/</v>
+        <f t="shared" si="2"/>
+        <v>https%3A%2F%2Fjaarverslag2013-a.rdw.nl%2F_trust%2F</v>
       </c>
       <c r="B79" t="s">
         <v>86</v>
@@ -9034,8 +9034,8 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="str">
-        <f t="shared" si="1"/>
-        <v>https://rpv.rdw.nl/</v>
+        <f t="shared" si="2"/>
+        <v>https%3A%2F%2Frpv.rdw.nl%2F</v>
       </c>
       <c r="B80" t="s">
         <v>115</v>
@@ -9047,8 +9047,8 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="str">
-        <f t="shared" si="1"/>
-        <v>https://crm.rdw.nl/</v>
+        <f t="shared" si="2"/>
+        <v>https%3A%2F%2Fcrm.rdw.nl%2F</v>
       </c>
       <c r="B81" t="s">
         <v>116</v>
@@ -9060,8 +9060,8 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="str">
-        <f t="shared" si="1"/>
-        <v>https://gpk.rdw.nl/</v>
+        <f t="shared" si="2"/>
+        <v>https%3A%2F%2Fgpk.rdw.nl%2F</v>
       </c>
       <c r="B82" t="s">
         <v>117</v>
@@ -9073,8 +9073,8 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="str">
-        <f t="shared" si="1"/>
-        <v>https://crwam.rdw.nl/</v>
+        <f t="shared" si="2"/>
+        <v>https%3A%2F%2Fcrwam.rdw.nl%2F</v>
       </c>
       <c r="B83" t="s">
         <v>118</v>
@@ -9086,8 +9086,8 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="str">
-        <f t="shared" si="1"/>
-        <v>https://gaikonline.rdw.nl/</v>
+        <f t="shared" si="2"/>
+        <v>https%3A%2F%2Fgaikonline.rdw.nl%2F</v>
       </c>
       <c r="B84" t="s">
         <v>119</v>
@@ -9099,8 +9099,8 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="str">
-        <f t="shared" si="1"/>
-        <v>https://inform.rdw.nl/</v>
+        <f t="shared" si="2"/>
+        <v>https%3A%2F%2Finform.rdw.nl%2F</v>
       </c>
       <c r="B85" t="s">
         <v>120</v>
@@ -9112,8 +9112,8 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="str">
-        <f t="shared" si="1"/>
-        <v>https://ddl-beheer.rdw.nl/</v>
+        <f>"https%3A%2F%2F"&amp;SUBSTITUTE(B86,"/","%2F")&amp;"%2F"</f>
+        <v>https%3A%2F%2Fddl-beheer.rdw.nl%2F</v>
       </c>
       <c r="B86" t="s">
         <v>121</v>

</xml_diff>